<commit_message>
Ajout de la récupération du prix / position / variation 1 jour et maj de la feuille excel
</commit_message>
<xml_diff>
--- a/src/main/resources/crypto.xlsx
+++ b/src/main/resources/crypto.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13935" windowHeight="5865"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13935" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="158">
   <si>
     <t>BTC</t>
   </si>
@@ -344,6 +343,156 @@
   </si>
   <si>
     <t>Date Maj</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/tierion/</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/bitcoin/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/ethereum/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/chainlink/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/crpt/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/ripio-credit-network/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/0x/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/enjin-coin/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/numeraire/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/status/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/streamr/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/crypto-com-coin/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/cardano/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/stellar/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/dash/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/icon/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/omg/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/cindicator/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/dragonchain/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/funfair/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/gas/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/gifto/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/power-ledger/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/quantstamp/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/vechain/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/zcash/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/cosmos/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/stacks/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/basic-attention-token/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/xrp/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/aave/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/uniswap/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/balancer/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/compound/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/curve-dao-token/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/synthetix-network-token/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/mirror-protocol/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/saffron-finance/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/rari-governance-token/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/yearn-finance/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/celsius/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/cover-protocol-new/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/armor/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/polkacover/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/ren/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/keeperdao/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/badger-dao/</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/fr/currencies/avalanche/</t>
+  </si>
+  <si>
+    <t>21/03/2021</t>
   </si>
 </sst>
 </file>
@@ -353,7 +502,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +514,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -391,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -401,12 +556,185 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -682,19 +1010,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CC59"/>
+  <dimension ref="A1:CD55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.42578125" style="5" collapsed="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="42" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.28515625" style="9" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="62.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="43" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -710,36 +1042,71 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" t="s">
         <v>107</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>48010</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="H2" s="10">
+        <v>-3.49E-2</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:81" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1493.95</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="H3" s="10">
+        <v>-4.0599999999999997E-2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:82" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -748,14 +1115,24 @@
       </c>
       <c r="C4"/>
       <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
+      <c r="E4">
+        <v>24.7</v>
+      </c>
+      <c r="F4" s="10"/>
       <c r="G4"/>
-      <c r="H4"/>
+      <c r="H4" s="10">
+        <v>-4.2300000000000004E-2</v>
+      </c>
       <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>157</v>
+      </c>
+      <c r="L4" t="s">
+        <v>112</v>
+      </c>
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
@@ -796,23 +1173,55 @@
       <c r="AX4"/>
       <c r="AY4"/>
       <c r="AZ4"/>
-    </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="BA4"/>
+    </row>
+    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>6.6889999999999996E-3</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="H5" s="10">
+        <v>-4.5899999999999996E-2</v>
+      </c>
+      <c r="J5">
+        <v>1202</v>
+      </c>
+      <c r="K5" t="s">
+        <v>157</v>
+      </c>
+      <c r="L5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="E6">
+        <v>0.38629999999999998</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="H6" s="10">
+        <v>-5.0599999999999999E-2</v>
+      </c>
+      <c r="J6">
+        <v>577</v>
+      </c>
+      <c r="K6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" t="s">
+        <v>113</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -843,7 +1252,7 @@
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
-      <c r="BP6" s="1"/>
+      <c r="AQ6" s="1"/>
       <c r="BQ6" s="1"/>
       <c r="BR6" s="1"/>
       <c r="BS6" s="1"/>
@@ -857,33 +1266,82 @@
       <c r="CA6" s="1"/>
       <c r="CB6" s="1"/>
       <c r="CC6" s="1"/>
-    </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="CD6" s="1"/>
+    </row>
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>0.12470000000000001</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="H7" s="10">
+        <v>-0.17269999999999999</v>
+      </c>
+      <c r="J7">
+        <v>422</v>
+      </c>
+      <c r="K7" t="s">
+        <v>157</v>
+      </c>
+      <c r="L7" t="s">
+        <v>114</v>
+      </c>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1.23</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="H8" s="10">
+        <v>-7.5499999999999998E-2</v>
+      </c>
+      <c r="J8">
+        <v>78</v>
+      </c>
+      <c r="K8" t="s">
+        <v>157</v>
+      </c>
+      <c r="L8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1.9</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="H9" s="10">
+        <v>-5.6100000000000004E-2</v>
+      </c>
+      <c r="J9">
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>157</v>
+      </c>
+      <c r="L9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -892,14 +1350,24 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2">
+        <v>42.51</v>
+      </c>
+      <c r="F10" s="10"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="10">
+        <v>-3.4099999999999998E-2</v>
+      </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="J10" s="2">
+        <v>160</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -956,8 +1424,9 @@
       <c r="BN10" s="2"/>
       <c r="BO10" s="2"/>
       <c r="BP10" s="2"/>
-    </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="BQ10" s="2"/>
+    </row>
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -966,14 +1435,24 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="2">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="F11" s="10"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="10">
+        <v>-6.93E-2</v>
+      </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="J11" s="2">
+        <v>130</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1030,364 +1509,998 @@
       <c r="BN11" s="2"/>
       <c r="BO11" s="2"/>
       <c r="BP11" s="2"/>
-    </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="BQ11" s="2"/>
+    </row>
+    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>0.1188</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="H12" s="10">
+        <v>-2.3099999999999999E-2</v>
+      </c>
+      <c r="J12">
+        <v>324</v>
+      </c>
+      <c r="K12" t="s">
+        <v>157</v>
+      </c>
+      <c r="L12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>0.1847</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="H13" s="10">
+        <v>-4.6500000000000007E-2</v>
+      </c>
+      <c r="J13">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
+        <v>157</v>
+      </c>
+      <c r="L13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="H14" s="10">
+        <v>-4.7699999999999992E-2</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14" t="s">
+        <v>157</v>
+      </c>
+      <c r="L14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>0.33560000000000001</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="H15" s="10">
+        <v>-2.3099999999999999E-2</v>
+      </c>
+      <c r="J15">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>157</v>
+      </c>
+      <c r="L15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>186.88</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="H16" s="10">
+        <v>-4.1500000000000002E-2</v>
+      </c>
+      <c r="J16">
+        <v>45</v>
+      </c>
+      <c r="K16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1.64</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="H17" s="10">
+        <v>-4.3899999999999995E-2</v>
+      </c>
+      <c r="J17">
+        <v>76</v>
+      </c>
+      <c r="K17" t="s">
+        <v>157</v>
+      </c>
+      <c r="L17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>4.7</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="H18" s="10">
+        <v>-5.8600000000000006E-2</v>
+      </c>
+      <c r="J18">
+        <v>90</v>
+      </c>
+      <c r="K18" t="s">
+        <v>157</v>
+      </c>
+      <c r="L18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>2.928E-2</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="H20" s="10">
+        <v>-2.1600000000000001E-2</v>
+      </c>
+      <c r="J20">
+        <v>435</v>
+      </c>
+      <c r="K20" t="s">
+        <v>157</v>
+      </c>
+      <c r="L20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="H21" s="10">
+        <v>-1.6899999999999998E-2</v>
+      </c>
+      <c r="J21">
+        <v>408</v>
+      </c>
+      <c r="K21" t="s">
+        <v>157</v>
+      </c>
+      <c r="L21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>3.1870000000000002E-2</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="H22" s="10">
+        <v>-5.4000000000000006E-2</v>
+      </c>
+      <c r="J22">
+        <v>128</v>
+      </c>
+      <c r="K22" t="s">
+        <v>157</v>
+      </c>
+      <c r="L22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="H23" s="10">
+        <v>-1.4199999999999999E-2</v>
+      </c>
+      <c r="J23">
+        <v>315</v>
+      </c>
+      <c r="K23" t="s">
+        <v>157</v>
+      </c>
+      <c r="L23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>3.5839999999999997E-2</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="H25" s="10">
+        <v>-3.7200000000000004E-2</v>
+      </c>
+      <c r="J25">
+        <v>620</v>
+      </c>
+      <c r="K25" t="s">
+        <v>157</v>
+      </c>
+      <c r="L25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>0.308</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="H26" s="10">
+        <v>-7.5199999999999989E-2</v>
+      </c>
+      <c r="J26">
+        <v>273</v>
+      </c>
+      <c r="K26" t="s">
+        <v>157</v>
+      </c>
+      <c r="L26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="H27" s="10">
+        <v>-9.1999999999999998E-2</v>
+      </c>
+      <c r="J27">
+        <v>453</v>
+      </c>
+      <c r="K27" t="s">
+        <v>157</v>
+      </c>
+      <c r="L27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>7.5569999999999998E-2</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="H28" s="10">
+        <v>-1.7299999999999999E-2</v>
+      </c>
+      <c r="J28">
+        <v>18</v>
+      </c>
+      <c r="K28" t="s">
+        <v>157</v>
+      </c>
+      <c r="L28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>123.75</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="H29" s="10">
+        <v>-6.2100000000000002E-2</v>
+      </c>
+      <c r="J29">
+        <v>57</v>
+      </c>
+      <c r="K29" t="s">
+        <v>157</v>
+      </c>
+      <c r="L29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>17.36</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="H30" s="10">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="J30">
+        <v>22</v>
+      </c>
+      <c r="K30" t="s">
+        <v>157</v>
+      </c>
+      <c r="L30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>186.88</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="H31" s="10">
+        <v>-4.1500000000000002E-2</v>
+      </c>
+      <c r="J31">
+        <v>45</v>
+      </c>
+      <c r="K31" t="s">
+        <v>157</v>
+      </c>
+      <c r="L31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>1.05</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="H32" s="10">
+        <v>-7.9500000000000001E-2</v>
+      </c>
+      <c r="J32">
+        <v>67</v>
+      </c>
+      <c r="K32" t="s">
+        <v>157</v>
+      </c>
+      <c r="L32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>0.9345</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="H33" s="10">
+        <v>-0.06</v>
+      </c>
+      <c r="J33">
+        <v>58</v>
+      </c>
+      <c r="K33" t="s">
+        <v>157</v>
+      </c>
+      <c r="L33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="H34" s="10">
+        <v>-0.02</v>
+      </c>
+      <c r="J34">
+        <v>7</v>
+      </c>
+      <c r="K34" t="s">
+        <v>157</v>
+      </c>
+      <c r="L34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>310.47000000000003</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="H35" s="10">
+        <v>-5.1299999999999998E-2</v>
+      </c>
+      <c r="J35">
+        <v>21</v>
+      </c>
+      <c r="K35" t="s">
+        <v>157</v>
+      </c>
+      <c r="L35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>27</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="H36" s="10">
+        <v>-2.7099999999999999E-2</v>
+      </c>
+      <c r="J36">
+        <v>8</v>
+      </c>
+      <c r="K36" t="s">
+        <v>157</v>
+      </c>
+      <c r="L36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>49.21</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="H37" s="10">
+        <v>-0.1018</v>
+      </c>
+      <c r="J37">
+        <v>125</v>
+      </c>
+      <c r="K37" t="s">
+        <v>157</v>
+      </c>
+      <c r="L37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="39" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>342.21</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="H38" s="10">
+        <v>-4.7599999999999996E-2</v>
+      </c>
+      <c r="J38">
+        <v>53</v>
+      </c>
+      <c r="K38" t="s">
+        <v>157</v>
+      </c>
+      <c r="L38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="40" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>2.19</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="H39" s="10">
+        <v>-9.3299999999999994E-2</v>
+      </c>
+      <c r="J39">
+        <v>99</v>
+      </c>
+      <c r="K39" t="s">
+        <v>157</v>
+      </c>
+      <c r="L39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>16.46</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="H40" s="10">
+        <v>-7.22E-2</v>
+      </c>
+      <c r="J40">
+        <v>44</v>
+      </c>
+      <c r="K40" t="s">
+        <v>157</v>
+      </c>
+      <c r="L40" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>6.16</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="H41" s="10">
+        <v>-8.1300000000000011E-2</v>
+      </c>
+      <c r="J41">
+        <v>232</v>
+      </c>
+      <c r="K41" t="s">
+        <v>157</v>
+      </c>
+      <c r="L41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="43" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>1356.63</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="H42" s="10">
+        <v>-0.1076</v>
+      </c>
+      <c r="J42">
+        <v>309</v>
+      </c>
+      <c r="K42" t="s">
+        <v>157</v>
+      </c>
+      <c r="L42" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="44" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>15.86</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="H43" s="10">
+        <v>-3.7699999999999997E-2</v>
+      </c>
+      <c r="J43">
+        <v>267</v>
+      </c>
+      <c r="K43" t="s">
+        <v>157</v>
+      </c>
+      <c r="L43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="45" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>29702.12</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="H44" s="10">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+      <c r="J44">
+        <v>73</v>
+      </c>
+      <c r="K44" t="s">
+        <v>157</v>
+      </c>
+      <c r="L44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="H45" s="10">
+        <v>-4.4800000000000006E-2</v>
+      </c>
+      <c r="J45">
+        <v>75</v>
+      </c>
+      <c r="K45" t="s">
+        <v>157</v>
+      </c>
+      <c r="L45" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="47" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>507.59</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="H46" s="10">
+        <v>-4.0099999999999997E-2</v>
+      </c>
+      <c r="J46">
+        <v>593</v>
+      </c>
+      <c r="K46" t="s">
+        <v>157</v>
+      </c>
+      <c r="L46" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>0.4919</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="H47" s="10">
+        <v>-6.9800000000000001E-2</v>
+      </c>
+      <c r="J47">
+        <v>884</v>
+      </c>
+      <c r="K47" t="s">
+        <v>157</v>
+      </c>
+      <c r="L47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="49" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>0.57689999999999997</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="H48" s="10">
+        <v>-0.18109999999999998</v>
+      </c>
+      <c r="J48">
+        <v>2481</v>
+      </c>
+      <c r="K48" t="s">
+        <v>157</v>
+      </c>
+      <c r="L48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="50" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>0.89280000000000004</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="H49" s="10">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="J49">
+        <v>81</v>
+      </c>
+      <c r="K49" t="s">
+        <v>157</v>
+      </c>
+      <c r="L49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="51" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>302.8</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="H50" s="10">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+      <c r="J50">
+        <v>854</v>
+      </c>
+      <c r="K50" t="s">
+        <v>157</v>
+      </c>
+      <c r="L50" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="52" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>36.9</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="H51" s="10">
+        <v>-4.9100000000000005E-2</v>
+      </c>
+      <c r="J51">
+        <v>131</v>
+      </c>
+      <c r="K51" t="s">
+        <v>157</v>
+      </c>
+      <c r="L51" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="53" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
+      <c r="E52">
+        <v>27.69</v>
+      </c>
+      <c r="F52" s="10"/>
+      <c r="H52" s="10">
+        <v>-8.9399999999999993E-2</v>
+      </c>
+      <c r="J52">
+        <v>24</v>
+      </c>
+      <c r="K52" t="s">
+        <v>157</v>
+      </c>
+      <c r="L52" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
-    </row>
-    <row r="57" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
-    </row>
-    <row r="58" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-    </row>
-    <row r="59" spans="1:81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H52">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F52">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
fix : correction gestion du fichier excel deja ouvert
</commit_message>
<xml_diff>
--- a/src/main/resources/crypto.xlsx
+++ b/src/main/resources/crypto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>ETH</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>02/04/21 23:13</t>
+  </si>
+  <si>
+    <t>02/04/21 23:25</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -337,6 +340,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -780,24 +790,24 @@
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="21" t="n">
-        <v>50191.43</v>
+        <v>50160.92</v>
       </c>
       <c r="J4" s="33" t="n">
         <f t="shared" ref="J4:J13" si="1">IF(I4&lt;&gt;"",(F4*I4)-G4,"")</f>
-        <v>3019.143</v>
+        <v>3016.0920000000006</v>
       </c>
       <c r="K4" s="34" t="n">
         <f t="shared" ref="K4:K13" si="2">IF(I4&lt;&gt;"",1/E4*I4-1,"")</f>
-        <v>1.5095715000000003</v>
-      </c>
-      <c r="L4" s="55" t="n">
-        <v>-0.0040999999999999995</v>
+        <v>1.5080460000000002</v>
+      </c>
+      <c r="L4" s="62" t="n">
+        <v>-0.0046</v>
       </c>
       <c r="M4" s="17" t="s">
         <v>11</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -822,24 +832,24 @@
       </c>
       <c r="H5" s="27"/>
       <c r="I5" s="28" t="n">
-        <v>1788.21</v>
+        <v>1780.45</v>
       </c>
       <c r="J5" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>38.821000000000026</v>
+        <v>38.045000000000016</v>
       </c>
       <c r="K5" s="23" t="n">
         <f t="shared" si="2"/>
-        <v>0.27729285714285723</v>
-      </c>
-      <c r="L5" s="56" t="n">
-        <v>0.0608</v>
+        <v>0.27174999999999994</v>
+      </c>
+      <c r="L5" s="63" t="n">
+        <v>0.0535</v>
       </c>
       <c r="M5" s="24" t="s">
         <v>12</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -874,14 +884,14 @@
         <f t="shared" si="2"/>
         <v>0.6799999999999999</v>
       </c>
-      <c r="L6" s="57" t="n">
-        <v>0.024</v>
+      <c r="L6" s="64" t="n">
+        <v>0.0199</v>
       </c>
       <c r="M6" s="24" t="s">
         <v>13</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
@@ -906,24 +916,24 @@
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="28" t="n">
-        <v>2.85</v>
+        <v>2.87</v>
       </c>
       <c r="J7" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>0.18500000000000003</v>
+        <v>0.18700000000000003</v>
       </c>
       <c r="K7" s="23" t="n">
         <f t="shared" si="2"/>
-        <v>1.85</v>
-      </c>
-      <c r="L7" s="58" t="n">
-        <v>-0.0088</v>
+        <v>1.87</v>
+      </c>
+      <c r="L7" s="65" t="n">
+        <v>-0.014199999999999999</v>
       </c>
       <c r="M7" s="24" t="s">
         <v>15</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
@@ -934,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>666.0</v>
+        <v>665.0</v>
       </c>
       <c r="E8" s="25">
         <v>800</v>
@@ -948,24 +958,24 @@
       </c>
       <c r="H8" s="27"/>
       <c r="I8" s="28" t="n">
-        <v>488.4</v>
+        <v>487.37</v>
       </c>
       <c r="J8" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>-31.159999999999997</v>
+        <v>-31.262999999999998</v>
       </c>
       <c r="K8" s="23" t="n">
         <f t="shared" si="2"/>
-        <v>-0.38950000000000007</v>
-      </c>
-      <c r="L8" s="59" t="n">
-        <v>0.0067</v>
+        <v>-0.39078749999999995</v>
+      </c>
+      <c r="L8" s="66" t="n">
+        <v>0.006</v>
       </c>
       <c r="M8" s="24" t="s">
         <v>16</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
@@ -990,24 +1000,24 @@
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="28" t="n">
-        <v>0.9211</v>
+        <v>0.9268</v>
       </c>
       <c r="J9" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>-0.007889999999999994</v>
+        <v>-0.007320000000000007</v>
       </c>
       <c r="K9" s="23" t="n">
         <f t="shared" si="2"/>
-        <v>-0.07889999999999997</v>
-      </c>
-      <c r="L9" s="60" t="n">
-        <v>0.020099999999999996</v>
+        <v>-0.07320000000000004</v>
+      </c>
+      <c r="L9" s="67" t="n">
+        <v>0.0282</v>
       </c>
       <c r="M9" s="24" t="s">
         <v>17</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
@@ -1032,24 +1042,24 @@
       </c>
       <c r="H10" s="27"/>
       <c r="I10" s="28" t="n">
-        <v>0.1937</v>
+        <v>0.1941</v>
       </c>
       <c r="J10" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>0.006870000000000001</v>
+        <v>0.0069099999999999995</v>
       </c>
       <c r="K10" s="23" t="n">
         <f t="shared" si="2"/>
-        <v>0.5496000000000001</v>
-      </c>
-      <c r="L10" s="61" t="n">
-        <v>0.0334</v>
+        <v>0.5528</v>
+      </c>
+      <c r="L10" s="68" t="n">
+        <v>0.035699999999999996</v>
       </c>
       <c r="M10" s="24" t="s">
         <v>14</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat : Ajout de la récupération des variations : 1jour, 7, 14, 30, 60, 90, 180, 360, début de l'année
</commit_message>
<xml_diff>
--- a/src/main/resources/crypto.xlsx
+++ b/src/main/resources/crypto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>ETH</t>
   </si>
@@ -123,25 +123,43 @@
     <t>Rang</t>
   </si>
   <si>
-    <t>Variation 24h</t>
-  </si>
-  <si>
-    <t>24/03/21 21:09</t>
-  </si>
-  <si>
-    <t>02/04/21 22:48</t>
-  </si>
-  <si>
-    <t>02/04/21 23:09</t>
-  </si>
-  <si>
-    <t>02/04/21 23:12</t>
-  </si>
-  <si>
-    <t>02/04/21 23:13</t>
-  </si>
-  <si>
-    <t>02/04/21 23:25</t>
+    <t>Variations</t>
+  </si>
+  <si>
+    <t>24h</t>
+  </si>
+  <si>
+    <t>7 jours</t>
+  </si>
+  <si>
+    <t>14 jours</t>
+  </si>
+  <si>
+    <t>30 jours</t>
+  </si>
+  <si>
+    <t>60 jours</t>
+  </si>
+  <si>
+    <t>90 jours</t>
+  </si>
+  <si>
+    <t>180 jours</t>
+  </si>
+  <si>
+    <t>360 jours</t>
+  </si>
+  <si>
+    <t>1er janvier</t>
+  </si>
+  <si>
+    <t>04/04/21 18:02</t>
+  </si>
+  <si>
+    <t>04/04/21 18:04</t>
+  </si>
+  <si>
+    <t>04/04/21 18:05</t>
   </si>
 </sst>
 </file>
@@ -149,7 +167,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +194,29 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -284,10 +325,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -315,7 +357,6 @@
     <xf numFmtId="17" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -326,20 +367,139 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -362,10 +522,227 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -675,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N27"/>
+  <dimension ref="B1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,21 +1071,30 @@
     <col min="9" max="9" customWidth="true" width="11.28515625" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
     <col min="11" max="11" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="12" max="19" customWidth="true" style="43" width="7.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="43" width="8.42578125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G1"/>
       <c r="H1"/>
       <c r="K1"/>
-      <c r="L1"/>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
       <c r="D2" s="7"/>
@@ -723,13 +1109,23 @@
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="6" t="s">
+      <c r="L2" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="2:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>18</v>
       </c>
@@ -758,17 +1154,41 @@
       <c r="K3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="12" t="s">
+      <c r="L3" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>20</v>
       </c>
@@ -790,420 +1210,703 @@
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="21" t="n">
-        <v>50160.92</v>
-      </c>
-      <c r="J4" s="33" t="n">
+        <v>49683.04</v>
+      </c>
+      <c r="J4" s="32" t="n">
         <f t="shared" ref="J4:J13" si="1">IF(I4&lt;&gt;"",(F4*I4)-G4,"")</f>
-        <v>3016.0920000000006</v>
-      </c>
-      <c r="K4" s="34" t="n">
+        <v>2968.304</v>
+      </c>
+      <c r="K4" s="51" t="n">
         <f t="shared" ref="K4:K13" si="2">IF(I4&lt;&gt;"",1/E4*I4-1,"")</f>
-        <v>1.5080460000000002</v>
-      </c>
-      <c r="L4" s="62" t="n">
-        <v>-0.0046</v>
-      </c>
-      <c r="M4" s="17" t="s">
+        <v>1.4841520000000004</v>
+      </c>
+      <c r="L4" s="124" t="n">
+        <v>0.009838757091655019</v>
+      </c>
+      <c r="M4" s="125" t="n">
+        <v>0.010430820875099955</v>
+      </c>
+      <c r="N4" s="126" t="n">
+        <v>0.0101397339616335</v>
+      </c>
+      <c r="O4" s="127" t="n">
+        <v>0.01270062580126196</v>
+      </c>
+      <c r="P4" s="128" t="n">
+        <v>0.01656714719328476</v>
+      </c>
+      <c r="Q4" s="129" t="n">
+        <v>0.018569792413467224</v>
+      </c>
+      <c r="R4" s="130" t="n">
+        <v>0.054267360460610765</v>
+      </c>
+      <c r="S4" s="131" t="n">
+        <v>0.07357648520053668</v>
+      </c>
+      <c r="T4" s="132" t="n">
+        <v>0.020902694801577824</v>
+      </c>
+      <c r="U4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="V4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>2.0</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>1400</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>0.1</v>
       </c>
-      <c r="G5" s="26" t="n">
+      <c r="G5" s="25" t="n">
         <f t="shared" si="0"/>
         <v>140.0</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28" t="n">
-        <v>1780.45</v>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27" t="n">
+        <v>1779.94</v>
       </c>
       <c r="J5" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>38.045000000000016</v>
-      </c>
-      <c r="K5" s="23" t="n">
+        <v>37.99400000000003</v>
+      </c>
+      <c r="K5" s="52" t="n">
         <f t="shared" si="2"/>
-        <v>0.27174999999999994</v>
-      </c>
-      <c r="L5" s="63" t="n">
-        <v>0.0535</v>
-      </c>
-      <c r="M5" s="24" t="s">
+        <v>0.27138571428571434</v>
+      </c>
+      <c r="L5" s="133" t="n">
+        <v>0.009766552397538684</v>
+      </c>
+      <c r="M5" s="134" t="n">
+        <v>0.01224097009323526</v>
+      </c>
+      <c r="N5" s="135" t="n">
+        <v>0.011730577304617039</v>
+      </c>
+      <c r="O5" s="136" t="n">
+        <v>0.014416006041594525</v>
+      </c>
+      <c r="P5" s="137" t="n">
+        <v>0.01410175820380534</v>
+      </c>
+      <c r="Q5" s="138" t="n">
+        <v>0.022229139685225264</v>
+      </c>
+      <c r="R5" s="139" t="n">
+        <v>0.05928454748614169</v>
+      </c>
+      <c r="S5" s="140" t="n">
+        <v>0.11197915491265316</v>
+      </c>
+      <c r="T5" s="141" t="n">
+        <v>0.029542153361183585</v>
+      </c>
+      <c r="U5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="V5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>71.0</v>
-      </c>
-      <c r="E6" s="25">
+        <v>73.0</v>
+      </c>
+      <c r="E6" s="24">
         <v>1</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>0.1</v>
       </c>
-      <c r="G6" s="26" t="n">
+      <c r="G6" s="25" t="n">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28" t="n">
-        <v>1.68</v>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27" t="n">
+        <v>1.55</v>
       </c>
       <c r="J6" s="22" t="n">
         <f>IF(I6&lt;&gt;"",(F6*I6)-G6,"")</f>
-        <v>0.068</v>
-      </c>
-      <c r="K6" s="23" t="n">
+        <v>0.05500000000000002</v>
+      </c>
+      <c r="K6" s="52" t="n">
         <f t="shared" si="2"/>
-        <v>0.6799999999999999</v>
-      </c>
-      <c r="L6" s="64" t="n">
-        <v>0.0199</v>
-      </c>
-      <c r="M6" s="24" t="s">
+        <v>0.55</v>
+      </c>
+      <c r="L6" s="142" t="n">
+        <v>0.009038770757500598</v>
+      </c>
+      <c r="M6" s="143" t="n">
+        <v>0.012762398410691116</v>
+      </c>
+      <c r="N6" s="144" t="n">
+        <v>0.012184870170915837</v>
+      </c>
+      <c r="O6" s="145" t="n">
+        <v>0.014145752430276772</v>
+      </c>
+      <c r="P6" s="146" t="n">
+        <v>0.027767919668662433</v>
+      </c>
+      <c r="Q6" s="147" t="n">
+        <v>0.047446096031143255</v>
+      </c>
+      <c r="R6" s="148" t="n">
+        <v>0.04839550480070918</v>
+      </c>
+      <c r="S6" s="149" t="n">
+        <v>0.09526423656408572</v>
+      </c>
+      <c r="T6" s="150" t="n">
+        <v>0.053087804179845995</v>
+      </c>
+      <c r="U6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="V6" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>99.0</v>
-      </c>
-      <c r="E7" s="25">
+        <v>103.0</v>
+      </c>
+      <c r="E7" s="24">
         <v>1</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <v>0.1</v>
       </c>
-      <c r="G7" s="26" t="n">
+      <c r="G7" s="25" t="n">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28" t="n">
-        <v>2.87</v>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27" t="n">
+        <v>2.61</v>
       </c>
       <c r="J7" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>0.18700000000000003</v>
-      </c>
-      <c r="K7" s="23" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="K7" s="52" t="n">
         <f t="shared" si="2"/>
-        <v>1.87</v>
-      </c>
-      <c r="L7" s="65" t="n">
-        <v>-0.014199999999999999</v>
-      </c>
-      <c r="M7" s="24" t="s">
+        <v>1.6099999999999999</v>
+      </c>
+      <c r="L7" s="151" t="n">
+        <v>0.00914325647946329</v>
+      </c>
+      <c r="M7" s="152" t="n">
+        <v>0.00974099907612782</v>
+      </c>
+      <c r="N7" s="153" t="n">
+        <v>0.011489356931052073</v>
+      </c>
+      <c r="O7" s="154" t="n">
+        <v>0.015747289334920235</v>
+      </c>
+      <c r="P7" s="155" t="n">
+        <v>0.012678422997512914</v>
+      </c>
+      <c r="Q7" s="156" t="n">
+        <v>0.045702740306540715</v>
+      </c>
+      <c r="R7" s="157" t="n">
+        <v>0.04873040491605767</v>
+      </c>
+      <c r="S7" s="158" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T7" s="159" t="n">
+        <v>0.049661541373610445</v>
+      </c>
+      <c r="U7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="V7" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>665.0</v>
-      </c>
-      <c r="E8" s="25">
+        <v>679.0</v>
+      </c>
+      <c r="E8" s="24">
         <v>800</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>0.1</v>
       </c>
-      <c r="G8" s="26" t="n">
+      <c r="G8" s="25" t="n">
         <f t="shared" si="0"/>
         <v>80.0</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28" t="n">
-        <v>487.37</v>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27" t="n">
+        <v>445.55</v>
       </c>
       <c r="J8" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>-31.262999999999998</v>
-      </c>
-      <c r="K8" s="23" t="n">
+        <v>-35.44499999999999</v>
+      </c>
+      <c r="K8" s="52" t="n">
         <f t="shared" si="2"/>
-        <v>-0.39078749999999995</v>
-      </c>
-      <c r="L8" s="66" t="n">
-        <v>0.006</v>
-      </c>
-      <c r="M8" s="24" t="s">
+        <v>-0.4430625</v>
+      </c>
+      <c r="L8" s="160" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="161" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="162" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="163" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="164" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q8" s="165" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" s="166" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="167" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T8" s="168" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="V8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>85.0</v>
-      </c>
-      <c r="E9" s="25">
+        <v>87.0</v>
+      </c>
+      <c r="E9" s="24">
         <v>1</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>0.1</v>
       </c>
-      <c r="G9" s="26" t="n">
+      <c r="G9" s="25" t="n">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28" t="n">
-        <v>0.9268</v>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27" t="n">
+        <v>0.9215</v>
       </c>
       <c r="J9" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>-0.007320000000000007</v>
-      </c>
-      <c r="K9" s="23" t="n">
+        <v>-0.007849999999999996</v>
+      </c>
+      <c r="K9" s="52" t="n">
         <f t="shared" si="2"/>
-        <v>-0.07320000000000004</v>
-      </c>
-      <c r="L9" s="67" t="n">
-        <v>0.0282</v>
-      </c>
-      <c r="M9" s="24" t="s">
+        <v>-0.07850000000000001</v>
+      </c>
+      <c r="L9" s="169" t="n">
+        <v>0.009803574767417769</v>
+      </c>
+      <c r="M9" s="170" t="n">
+        <v>0.011089608622740528</v>
+      </c>
+      <c r="N9" s="171" t="n">
+        <v>0.010144444449214847</v>
+      </c>
+      <c r="O9" s="172" t="n">
+        <v>0.011181638553066607</v>
+      </c>
+      <c r="P9" s="173" t="n">
+        <v>0.016863064486737543</v>
+      </c>
+      <c r="Q9" s="174" t="n">
+        <v>0.03401611910004902</v>
+      </c>
+      <c r="R9" s="175" t="n">
+        <v>0.04354197190935634</v>
+      </c>
+      <c r="S9" s="176" t="n">
+        <v>0.1885830607593543</v>
+      </c>
+      <c r="T9" s="177" t="n">
+        <v>0.03452195890669349</v>
+      </c>
+      <c r="U9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="V9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>24.0</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>0.125</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>0.1</v>
       </c>
-      <c r="G10" s="26" t="n">
+      <c r="G10" s="25" t="n">
         <f t="shared" si="0"/>
         <v>0.0125</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28" t="n">
-        <v>0.1941</v>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27" t="n">
+        <v>0.1906</v>
       </c>
       <c r="J10" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>0.0069099999999999995</v>
-      </c>
-      <c r="K10" s="23" t="n">
+        <v>0.00656</v>
+      </c>
+      <c r="K10" s="52" t="n">
         <f t="shared" si="2"/>
-        <v>0.5528</v>
-      </c>
-      <c r="L10" s="68" t="n">
-        <v>0.035699999999999996</v>
-      </c>
-      <c r="M10" s="24" t="s">
+        <v>0.5247999999999999</v>
+      </c>
+      <c r="L10" s="178" t="n">
+        <v>0.009715521279259915</v>
+      </c>
+      <c r="M10" s="179" t="n">
+        <v>0.011009220308649788</v>
+      </c>
+      <c r="N10" s="180" t="n">
+        <v>0.010385016023763707</v>
+      </c>
+      <c r="O10" s="181" t="n">
+        <v>0.015647735807109556</v>
+      </c>
+      <c r="P10" s="182" t="n">
+        <v>0.036127393605678786</v>
+      </c>
+      <c r="Q10" s="183" t="n">
+        <v>0.039335806852520444</v>
+      </c>
+      <c r="R10" s="184" t="n">
+        <v>0.014979302470626106</v>
+      </c>
+      <c r="S10" s="185" t="n">
+        <v>0.03846606378948851</v>
+      </c>
+      <c r="T10" s="186" t="n">
+        <v>0.039688852721455885</v>
+      </c>
+      <c r="U10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="31"/>
+      <c r="V10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="27"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="27"/>
       <c r="J11" s="22" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K11" s="23" t="str">
+      <c r="K11" s="52" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L11" s="23"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="4" t="s">
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="31"/>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="27"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
       <c r="J12" s="22" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K12" s="23" t="str">
+      <c r="K12" s="52" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="4" t="s">
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="38" t="str">
+    <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="39" t="str">
+      <c r="K13" s="53" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L13" s="39"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="30" t="s">
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N14" t="s">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N15" t="s">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N16" t="s">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N17" t="s">
+    <row r="17" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N19" t="s">
+    <row r="19" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N21" t="s">
+    <row r="21" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N22" t="s">
+    <row r="22" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N23" t="s">
+    <row r="23" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N24" t="s">
+    <row r="24" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N25" t="s">
+    <row r="25" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N26" t="s">
+    <row r="26" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N27" t="s">
+    <row r="27" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J4:L13">
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="38" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M13">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R13">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4:S13">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T13">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P13">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:Q13">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N13">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:O13">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="U6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refacto : suppression demarrage springboot
</commit_message>
<xml_diff>
--- a/src/main/resources/crypto.xlsx
+++ b/src/main/resources/crypto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>ETH</t>
   </si>
@@ -153,20 +153,16 @@
     <t>1er janvier</t>
   </si>
   <si>
-    <t>04/04/21 18:02</t>
-  </si>
-  <si>
-    <t>04/04/21 18:04</t>
-  </si>
-  <si>
     <t>04/04/21 18:05</t>
+  </si>
+  <si>
+    <t>04/04/21 18:12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -329,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -451,76 +447,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1044,7 +970,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1052,32 +978,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V27"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="1.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="8.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="12" max="19" customWidth="true" style="43" width="7.7109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="43" width="8.42578125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="19" width="7.7109375" style="43" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.42578125" style="43" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="7.7109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1195,8 +1120,8 @@
       <c r="C4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>1.0</v>
+      <c r="D4" s="3">
+        <v>1</v>
       </c>
       <c r="E4" s="18">
         <v>20000</v>
@@ -1204,54 +1129,54 @@
       <c r="F4" s="18">
         <v>0.1</v>
       </c>
-      <c r="G4" s="19" t="n">
+      <c r="G4" s="19">
         <f t="shared" ref="G4:G10" si="0">E4*F4</f>
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="H4" s="20"/>
-      <c r="I4" s="21" t="n">
-        <v>49683.04</v>
-      </c>
-      <c r="J4" s="32" t="n">
+      <c r="I4" s="21">
+        <v>49714.5</v>
+      </c>
+      <c r="J4" s="32">
         <f t="shared" ref="J4:J13" si="1">IF(I4&lt;&gt;"",(F4*I4)-G4,"")</f>
-        <v>2968.304</v>
-      </c>
-      <c r="K4" s="51" t="n">
+        <v>2971.4500000000007</v>
+      </c>
+      <c r="K4" s="51">
         <f t="shared" ref="K4:K13" si="2">IF(I4&lt;&gt;"",1/E4*I4-1,"")</f>
-        <v>1.4841520000000004</v>
-      </c>
-      <c r="L4" s="124" t="n">
-        <v>0.009838757091655019</v>
-      </c>
-      <c r="M4" s="125" t="n">
-        <v>0.010430820875099955</v>
-      </c>
-      <c r="N4" s="126" t="n">
-        <v>0.0101397339616335</v>
-      </c>
-      <c r="O4" s="127" t="n">
-        <v>0.01270062580126196</v>
-      </c>
-      <c r="P4" s="128" t="n">
-        <v>0.01656714719328476</v>
-      </c>
-      <c r="Q4" s="129" t="n">
-        <v>0.018569792413467224</v>
-      </c>
-      <c r="R4" s="130" t="n">
-        <v>0.054267360460610765</v>
-      </c>
-      <c r="S4" s="131" t="n">
-        <v>0.07357648520053668</v>
-      </c>
-      <c r="T4" s="132" t="n">
-        <v>0.020902694801577824</v>
+        <v>1.485725</v>
+      </c>
+      <c r="L4" s="99">
+        <v>9.8449871310830293E-3</v>
+      </c>
+      <c r="M4" s="100">
+        <v>1.0437425817646357E-2</v>
+      </c>
+      <c r="N4" s="101">
+        <v>1.0146154583850518E-2</v>
+      </c>
+      <c r="O4" s="102">
+        <v>1.2708668016225208E-2</v>
+      </c>
+      <c r="P4" s="103">
+        <v>1.6577637743997856E-2</v>
+      </c>
+      <c r="Q4" s="104">
+        <v>1.858155106731223E-2</v>
+      </c>
+      <c r="R4" s="105">
+        <v>5.4301723316830738E-2</v>
+      </c>
+      <c r="S4" s="106">
+        <v>7.3623074866233637E-2</v>
+      </c>
+      <c r="T4" s="107">
+        <v>2.0915930682040406E-2</v>
       </c>
       <c r="U4" s="17" t="s">
         <v>11</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
@@ -1261,8 +1186,8 @@
       <c r="C5" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="n">
-        <v>2.0</v>
+      <c r="D5" s="4">
+        <v>2</v>
       </c>
       <c r="E5" s="24">
         <v>1400</v>
@@ -1270,54 +1195,54 @@
       <c r="F5" s="24">
         <v>0.1</v>
       </c>
-      <c r="G5" s="25" t="n">
+      <c r="G5" s="25">
         <f t="shared" si="0"/>
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="H5" s="26"/>
-      <c r="I5" s="27" t="n">
-        <v>1779.94</v>
-      </c>
-      <c r="J5" s="22" t="n">
+      <c r="I5" s="27">
+        <v>1780.3</v>
+      </c>
+      <c r="J5" s="22">
         <f t="shared" si="1"/>
-        <v>37.99400000000003</v>
-      </c>
-      <c r="K5" s="52" t="n">
+        <v>38.03</v>
+      </c>
+      <c r="K5" s="52">
         <f t="shared" si="2"/>
-        <v>0.27138571428571434</v>
-      </c>
-      <c r="L5" s="133" t="n">
-        <v>0.009766552397538684</v>
-      </c>
-      <c r="M5" s="134" t="n">
-        <v>0.01224097009323526</v>
-      </c>
-      <c r="N5" s="135" t="n">
-        <v>0.011730577304617039</v>
-      </c>
-      <c r="O5" s="136" t="n">
-        <v>0.014416006041594525</v>
-      </c>
-      <c r="P5" s="137" t="n">
-        <v>0.01410175820380534</v>
-      </c>
-      <c r="Q5" s="138" t="n">
-        <v>0.022229139685225264</v>
-      </c>
-      <c r="R5" s="139" t="n">
-        <v>0.05928454748614169</v>
-      </c>
-      <c r="S5" s="140" t="n">
-        <v>0.11197915491265316</v>
-      </c>
-      <c r="T5" s="141" t="n">
-        <v>0.029542153361183585</v>
+        <v>0.27164285714285707</v>
+      </c>
+      <c r="L5" s="108">
+        <v>9.7685277219109173E-3</v>
+      </c>
+      <c r="M5" s="109">
+        <v>1.2243445878505304E-2</v>
+      </c>
+      <c r="N5" s="110">
+        <v>1.1732949860899644E-2</v>
+      </c>
+      <c r="O5" s="111">
+        <v>1.4418921736603892E-2</v>
+      </c>
+      <c r="P5" s="112">
+        <v>1.4104610340929833E-2</v>
+      </c>
+      <c r="Q5" s="113">
+        <v>2.2233635617833487E-2</v>
+      </c>
+      <c r="R5" s="114">
+        <v>5.9296538023516546E-2</v>
+      </c>
+      <c r="S5" s="115">
+        <v>0.11200180314560965</v>
+      </c>
+      <c r="T5" s="116">
+        <v>2.9548128380122437E-2</v>
       </c>
       <c r="U5" s="23" t="s">
         <v>12</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
@@ -1327,8 +1252,8 @@
       <c r="C6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="n">
-        <v>73.0</v>
+      <c r="D6" s="4">
+        <v>73</v>
       </c>
       <c r="E6" s="24">
         <v>1</v>
@@ -1336,54 +1261,54 @@
       <c r="F6" s="24">
         <v>0.1</v>
       </c>
-      <c r="G6" s="25" t="n">
+      <c r="G6" s="25">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="H6" s="26"/>
-      <c r="I6" s="27" t="n">
+      <c r="I6" s="27">
         <v>1.55</v>
       </c>
-      <c r="J6" s="22" t="n">
+      <c r="J6" s="22">
         <f>IF(I6&lt;&gt;"",(F6*I6)-G6,"")</f>
-        <v>0.05500000000000002</v>
-      </c>
-      <c r="K6" s="52" t="n">
+        <v>5.5000000000000021E-2</v>
+      </c>
+      <c r="K6" s="52">
         <f t="shared" si="2"/>
-        <v>0.55</v>
-      </c>
-      <c r="L6" s="142" t="n">
-        <v>0.009038770757500598</v>
-      </c>
-      <c r="M6" s="143" t="n">
-        <v>0.012762398410691116</v>
-      </c>
-      <c r="N6" s="144" t="n">
-        <v>0.012184870170915837</v>
-      </c>
-      <c r="O6" s="145" t="n">
-        <v>0.014145752430276772</v>
-      </c>
-      <c r="P6" s="146" t="n">
-        <v>0.027767919668662433</v>
-      </c>
-      <c r="Q6" s="147" t="n">
-        <v>0.047446096031143255</v>
-      </c>
-      <c r="R6" s="148" t="n">
-        <v>0.04839550480070918</v>
-      </c>
-      <c r="S6" s="149" t="n">
-        <v>0.09526423656408572</v>
-      </c>
-      <c r="T6" s="150" t="n">
-        <v>0.053087804179845995</v>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L6" s="54">
+        <v>9.0387707575005985E-3</v>
+      </c>
+      <c r="M6" s="55">
+        <v>1.2762398410691116E-2</v>
+      </c>
+      <c r="N6" s="56">
+        <v>1.2184870170915837E-2</v>
+      </c>
+      <c r="O6" s="57">
+        <v>1.4145752430276772E-2</v>
+      </c>
+      <c r="P6" s="58">
+        <v>2.7767919668662433E-2</v>
+      </c>
+      <c r="Q6" s="59">
+        <v>4.7446096031143255E-2</v>
+      </c>
+      <c r="R6" s="60">
+        <v>4.8395504800709178E-2</v>
+      </c>
+      <c r="S6" s="61">
+        <v>9.5264236564085725E-2</v>
+      </c>
+      <c r="T6" s="62">
+        <v>5.3087804179845995E-2</v>
       </c>
       <c r="U6" s="50" t="s">
         <v>13</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
@@ -1393,8 +1318,8 @@
       <c r="C7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4" t="n">
-        <v>103.0</v>
+      <c r="D7" s="4">
+        <v>103</v>
       </c>
       <c r="E7" s="24">
         <v>1</v>
@@ -1402,54 +1327,54 @@
       <c r="F7" s="24">
         <v>0.1</v>
       </c>
-      <c r="G7" s="25" t="n">
+      <c r="G7" s="25">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="H7" s="26"/>
-      <c r="I7" s="27" t="n">
+      <c r="I7" s="27">
         <v>2.61</v>
       </c>
-      <c r="J7" s="22" t="n">
+      <c r="J7" s="22">
         <f t="shared" si="1"/>
         <v>0.161</v>
       </c>
-      <c r="K7" s="52" t="n">
+      <c r="K7" s="52">
         <f t="shared" si="2"/>
         <v>1.6099999999999999</v>
       </c>
-      <c r="L7" s="151" t="n">
-        <v>0.00914325647946329</v>
-      </c>
-      <c r="M7" s="152" t="n">
-        <v>0.00974099907612782</v>
-      </c>
-      <c r="N7" s="153" t="n">
-        <v>0.011489356931052073</v>
-      </c>
-      <c r="O7" s="154" t="n">
-        <v>0.015747289334920235</v>
-      </c>
-      <c r="P7" s="155" t="n">
-        <v>0.012678422997512914</v>
-      </c>
-      <c r="Q7" s="156" t="n">
-        <v>0.045702740306540715</v>
-      </c>
-      <c r="R7" s="157" t="n">
-        <v>0.04873040491605767</v>
-      </c>
-      <c r="S7" s="158" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T7" s="159" t="n">
-        <v>0.049661541373610445</v>
+      <c r="L7" s="63">
+        <v>9.1432564794632892E-3</v>
+      </c>
+      <c r="M7" s="64">
+        <v>9.7409990761278195E-3</v>
+      </c>
+      <c r="N7" s="65">
+        <v>1.1489356931052073E-2</v>
+      </c>
+      <c r="O7" s="66">
+        <v>1.5747289334920235E-2</v>
+      </c>
+      <c r="P7" s="67">
+        <v>1.2678422997512914E-2</v>
+      </c>
+      <c r="Q7" s="68">
+        <v>4.5702740306540715E-2</v>
+      </c>
+      <c r="R7" s="69">
+        <v>4.8730404916057672E-2</v>
+      </c>
+      <c r="S7" s="70">
+        <v>0</v>
+      </c>
+      <c r="T7" s="71">
+        <v>4.9661541373610445E-2</v>
       </c>
       <c r="U7" s="23" t="s">
         <v>15</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
@@ -1459,8 +1384,8 @@
       <c r="C8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4" t="n">
-        <v>679.0</v>
+      <c r="D8" s="4">
+        <v>679</v>
       </c>
       <c r="E8" s="24">
         <v>800</v>
@@ -1468,54 +1393,54 @@
       <c r="F8" s="24">
         <v>0.1</v>
       </c>
-      <c r="G8" s="25" t="n">
+      <c r="G8" s="25">
         <f t="shared" si="0"/>
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="H8" s="26"/>
-      <c r="I8" s="27" t="n">
+      <c r="I8" s="27">
         <v>445.55</v>
       </c>
-      <c r="J8" s="22" t="n">
+      <c r="J8" s="22">
         <f t="shared" si="1"/>
-        <v>-35.44499999999999</v>
-      </c>
-      <c r="K8" s="52" t="n">
+        <v>-35.444999999999993</v>
+      </c>
+      <c r="K8" s="52">
         <f t="shared" si="2"/>
-        <v>-0.4430625</v>
-      </c>
-      <c r="L8" s="160" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M8" s="161" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N8" s="162" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O8" s="163" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P8" s="164" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q8" s="165" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R8" s="166" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S8" s="167" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T8" s="168" t="n">
-        <v>0.0</v>
+        <v>-0.44306250000000003</v>
+      </c>
+      <c r="L8" s="72">
+        <v>0</v>
+      </c>
+      <c r="M8" s="73">
+        <v>0</v>
+      </c>
+      <c r="N8" s="74">
+        <v>0</v>
+      </c>
+      <c r="O8" s="75">
+        <v>0</v>
+      </c>
+      <c r="P8" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="77">
+        <v>0</v>
+      </c>
+      <c r="R8" s="78">
+        <v>0</v>
+      </c>
+      <c r="S8" s="79">
+        <v>0</v>
+      </c>
+      <c r="T8" s="80">
+        <v>0</v>
       </c>
       <c r="U8" s="23" t="s">
         <v>16</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
@@ -1525,8 +1450,8 @@
       <c r="C9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="n">
-        <v>87.0</v>
+      <c r="D9" s="4">
+        <v>87</v>
       </c>
       <c r="E9" s="24">
         <v>1</v>
@@ -1534,54 +1459,54 @@
       <c r="F9" s="24">
         <v>0.1</v>
       </c>
-      <c r="G9" s="25" t="n">
+      <c r="G9" s="25">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="H9" s="26"/>
-      <c r="I9" s="27" t="n">
-        <v>0.9215</v>
-      </c>
-      <c r="J9" s="22" t="n">
+      <c r="I9" s="27">
+        <v>0.92149999999999999</v>
+      </c>
+      <c r="J9" s="22">
         <f t="shared" si="1"/>
-        <v>-0.007849999999999996</v>
-      </c>
-      <c r="K9" s="52" t="n">
+        <v>-7.8499999999999959E-3</v>
+      </c>
+      <c r="K9" s="52">
         <f t="shared" si="2"/>
-        <v>-0.07850000000000001</v>
-      </c>
-      <c r="L9" s="169" t="n">
-        <v>0.009803574767417769</v>
-      </c>
-      <c r="M9" s="170" t="n">
-        <v>0.011089608622740528</v>
-      </c>
-      <c r="N9" s="171" t="n">
-        <v>0.010144444449214847</v>
-      </c>
-      <c r="O9" s="172" t="n">
-        <v>0.011181638553066607</v>
-      </c>
-      <c r="P9" s="173" t="n">
-        <v>0.016863064486737543</v>
-      </c>
-      <c r="Q9" s="174" t="n">
-        <v>0.03401611910004902</v>
-      </c>
-      <c r="R9" s="175" t="n">
-        <v>0.04354197190935634</v>
-      </c>
-      <c r="S9" s="176" t="n">
+        <v>-7.8500000000000014E-2</v>
+      </c>
+      <c r="L9" s="81">
+        <v>9.8035747674177689E-3</v>
+      </c>
+      <c r="M9" s="82">
+        <v>1.1089608622740528E-2</v>
+      </c>
+      <c r="N9" s="83">
+        <v>1.0144444449214847E-2</v>
+      </c>
+      <c r="O9" s="84">
+        <v>1.1181638553066607E-2</v>
+      </c>
+      <c r="P9" s="85">
+        <v>1.6863064486737543E-2</v>
+      </c>
+      <c r="Q9" s="86">
+        <v>3.4016119100049022E-2</v>
+      </c>
+      <c r="R9" s="87">
+        <v>4.3541971909356339E-2</v>
+      </c>
+      <c r="S9" s="88">
         <v>0.1885830607593543</v>
       </c>
-      <c r="T9" s="177" t="n">
-        <v>0.03452195890669349</v>
+      <c r="T9" s="89">
+        <v>3.452195890669349E-2</v>
       </c>
       <c r="U9" s="23" t="s">
         <v>17</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
@@ -1591,8 +1516,8 @@
       <c r="C10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="n">
-        <v>24.0</v>
+      <c r="D10" s="4">
+        <v>24</v>
       </c>
       <c r="E10" s="24">
         <v>0.125</v>
@@ -1600,54 +1525,54 @@
       <c r="F10" s="24">
         <v>0.1</v>
       </c>
-      <c r="G10" s="25" t="n">
+      <c r="G10" s="25">
         <f t="shared" si="0"/>
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="H10" s="26"/>
-      <c r="I10" s="27" t="n">
-        <v>0.1906</v>
-      </c>
-      <c r="J10" s="22" t="n">
+      <c r="I10" s="27">
+        <v>0.19059999999999999</v>
+      </c>
+      <c r="J10" s="22">
         <f t="shared" si="1"/>
-        <v>0.00656</v>
-      </c>
-      <c r="K10" s="52" t="n">
+        <v>6.5599999999999999E-3</v>
+      </c>
+      <c r="K10" s="52">
         <f t="shared" si="2"/>
-        <v>0.5247999999999999</v>
-      </c>
-      <c r="L10" s="178" t="n">
-        <v>0.009715521279259915</v>
-      </c>
-      <c r="M10" s="179" t="n">
-        <v>0.011009220308649788</v>
-      </c>
-      <c r="N10" s="180" t="n">
-        <v>0.010385016023763707</v>
-      </c>
-      <c r="O10" s="181" t="n">
-        <v>0.015647735807109556</v>
-      </c>
-      <c r="P10" s="182" t="n">
-        <v>0.036127393605678786</v>
-      </c>
-      <c r="Q10" s="183" t="n">
-        <v>0.039335806852520444</v>
-      </c>
-      <c r="R10" s="184" t="n">
-        <v>0.014979302470626106</v>
-      </c>
-      <c r="S10" s="185" t="n">
-        <v>0.03846606378948851</v>
-      </c>
-      <c r="T10" s="186" t="n">
-        <v>0.039688852721455885</v>
+        <v>0.52479999999999993</v>
+      </c>
+      <c r="L10" s="90">
+        <v>9.7155212792599151E-3</v>
+      </c>
+      <c r="M10" s="91">
+        <v>1.1009220308649788E-2</v>
+      </c>
+      <c r="N10" s="92">
+        <v>1.0385016023763707E-2</v>
+      </c>
+      <c r="O10" s="93">
+        <v>1.5647735807109556E-2</v>
+      </c>
+      <c r="P10" s="94">
+        <v>3.6127393605678786E-2</v>
+      </c>
+      <c r="Q10" s="95">
+        <v>3.9335806852520444E-2</v>
+      </c>
+      <c r="R10" s="96">
+        <v>1.4979302470626106E-2</v>
+      </c>
+      <c r="S10" s="97">
+        <v>3.8466063789488511E-2</v>
+      </c>
+      <c r="T10" s="98">
+        <v>3.9688852721455885E-2</v>
       </c>
       <c r="U10" s="23" t="s">
         <v>14</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fichier crypto avec les variations
</commit_message>
<xml_diff>
--- a/src/main/resources/crypto.xlsx
+++ b/src/main/resources/crypto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>ETH</t>
   </si>
@@ -153,16 +153,17 @@
     <t>1er janvier</t>
   </si>
   <si>
-    <t>04/04/21 18:05</t>
-  </si>
-  <si>
-    <t>04/04/21 18:12</t>
+    <t>07/04/21 21:41</t>
+  </si>
+  <si>
+    <t>07/04/21 21:42</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,7 +196,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -203,16 +212,8 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,9 +324,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -368,85 +369,86 @@
     <xf numFmtId="17" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -970,7 +972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -978,46 +980,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="B1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="19" width="7.7109375" style="43" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.42578125" style="43" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="7.7109375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="1.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="8.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="12" max="20" customWidth="true" style="54" width="8.42578125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G1"/>
       <c r="H1"/>
       <c r="K1"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
     </row>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1034,16 +1035,16 @@
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="11"/>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
       <c r="T2" s="45"/>
       <c r="U2" s="6" t="s">
         <v>26</v>
@@ -1082,28 +1083,28 @@
       <c r="L3" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="O3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="P3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="40" t="s">
+      <c r="Q3" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="40" t="s">
+      <c r="R3" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="47" t="s">
+      <c r="T3" s="48" t="s">
         <v>43</v>
       </c>
       <c r="U3" s="12" t="s">
@@ -1120,8 +1121,8 @@
       <c r="C4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
+      <c r="D4" s="3" t="n">
+        <v>1.0</v>
       </c>
       <c r="E4" s="18">
         <v>20000</v>
@@ -1129,48 +1130,48 @@
       <c r="F4" s="18">
         <v>0.1</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="19" t="n">
         <f t="shared" ref="G4:G10" si="0">E4*F4</f>
-        <v>2000</v>
+        <v>2000.0</v>
       </c>
       <c r="H4" s="20"/>
-      <c r="I4" s="21">
-        <v>49714.5</v>
-      </c>
-      <c r="J4" s="32">
+      <c r="I4" s="21" t="n">
+        <v>47010.35</v>
+      </c>
+      <c r="J4" s="32" t="n">
         <f t="shared" ref="J4:J13" si="1">IF(I4&lt;&gt;"",(F4*I4)-G4,"")</f>
-        <v>2971.4500000000007</v>
-      </c>
-      <c r="K4" s="51">
+        <v>2701.035</v>
+      </c>
+      <c r="K4" s="39" t="n">
         <f t="shared" ref="K4:K13" si="2">IF(I4&lt;&gt;"",1/E4*I4-1,"")</f>
-        <v>1.485725</v>
-      </c>
-      <c r="L4" s="99">
-        <v>9.8449871310830293E-3</v>
-      </c>
-      <c r="M4" s="100">
-        <v>1.0437425817646357E-2</v>
-      </c>
-      <c r="N4" s="101">
-        <v>1.0146154583850518E-2</v>
-      </c>
-      <c r="O4" s="102">
-        <v>1.2708668016225208E-2</v>
-      </c>
-      <c r="P4" s="103">
-        <v>1.6577637743997856E-2</v>
-      </c>
-      <c r="Q4" s="104">
-        <v>1.858155106731223E-2</v>
-      </c>
-      <c r="R4" s="105">
-        <v>5.4301723316830738E-2</v>
-      </c>
-      <c r="S4" s="106">
-        <v>7.3623074866233637E-2</v>
-      </c>
-      <c r="T4" s="107">
-        <v>2.0915930682040406E-2</v>
+        <v>1.3505175</v>
+      </c>
+      <c r="L4" s="55" t="n">
+        <v>-0.059357373475232435</v>
+      </c>
+      <c r="M4" s="56" t="n">
+        <v>-0.06460256583708386</v>
+      </c>
+      <c r="N4" s="57" t="n">
+        <v>0.03109184085750627</v>
+      </c>
+      <c r="O4" s="58" t="n">
+        <v>0.0880861136118746</v>
+      </c>
+      <c r="P4" s="59" t="n">
+        <v>0.4630739176408079</v>
+      </c>
+      <c r="Q4" s="60" t="n">
+        <v>0.5619458247977889</v>
+      </c>
+      <c r="R4" s="61" t="n">
+        <v>4.0676405613264635</v>
+      </c>
+      <c r="S4" s="62" t="n">
+        <v>6.494903400209579</v>
+      </c>
+      <c r="T4" s="63" t="n">
+        <v>0.9778238178769939</v>
       </c>
       <c r="U4" s="17" t="s">
         <v>11</v>
@@ -1186,8 +1187,8 @@
       <c r="C5" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4">
-        <v>2</v>
+      <c r="D5" s="4" t="n">
+        <v>2.0</v>
       </c>
       <c r="E5" s="24">
         <v>1400</v>
@@ -1195,48 +1196,48 @@
       <c r="F5" s="24">
         <v>0.1</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="25" t="n">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>140.0</v>
       </c>
       <c r="H5" s="26"/>
-      <c r="I5" s="27">
-        <v>1780.3</v>
-      </c>
-      <c r="J5" s="22">
+      <c r="I5" s="27" t="n">
+        <v>1657.69</v>
+      </c>
+      <c r="J5" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>38.03</v>
-      </c>
-      <c r="K5" s="52">
+        <v>25.769000000000005</v>
+      </c>
+      <c r="K5" s="40" t="n">
         <f t="shared" si="2"/>
-        <v>0.27164285714285707</v>
-      </c>
-      <c r="L5" s="108">
-        <v>9.7685277219109173E-3</v>
-      </c>
-      <c r="M5" s="109">
-        <v>1.2243445878505304E-2</v>
-      </c>
-      <c r="N5" s="110">
-        <v>1.1732949860899644E-2</v>
-      </c>
-      <c r="O5" s="111">
-        <v>1.4418921736603892E-2</v>
-      </c>
-      <c r="P5" s="112">
-        <v>1.4104610340929833E-2</v>
-      </c>
-      <c r="Q5" s="113">
-        <v>2.2233635617833487E-2</v>
-      </c>
-      <c r="R5" s="114">
-        <v>5.9296538023516546E-2</v>
-      </c>
-      <c r="S5" s="115">
-        <v>0.11200180314560965</v>
-      </c>
-      <c r="T5" s="116">
-        <v>2.9548128380122437E-2</v>
+        <v>0.1840642857142858</v>
+      </c>
+      <c r="L5" s="64" t="n">
+        <v>-0.07068063154096606</v>
+      </c>
+      <c r="M5" s="65" t="n">
+        <v>0.05271816359088433</v>
+      </c>
+      <c r="N5" s="66" t="n">
+        <v>0.1820692371549498</v>
+      </c>
+      <c r="O5" s="67" t="n">
+        <v>0.13441808662043842</v>
+      </c>
+      <c r="P5" s="68" t="n">
+        <v>0.1556354732714378</v>
+      </c>
+      <c r="Q5" s="69" t="n">
+        <v>0.6968970465409504</v>
+      </c>
+      <c r="R5" s="70" t="n">
+        <v>4.560949774605982</v>
+      </c>
+      <c r="S5" s="71" t="n">
+        <v>10.457542135724795</v>
+      </c>
+      <c r="T5" s="72" t="n">
+        <v>1.7513136513197305</v>
       </c>
       <c r="U5" s="23" t="s">
         <v>12</v>
@@ -1252,8 +1253,8 @@
       <c r="C6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
-        <v>73</v>
+      <c r="D6" s="4" t="n">
+        <v>81.0</v>
       </c>
       <c r="E6" s="24">
         <v>1</v>
@@ -1261,54 +1262,54 @@
       <c r="F6" s="24">
         <v>0.1</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="25" t="n">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="H6" s="26"/>
-      <c r="I6" s="27">
-        <v>1.55</v>
-      </c>
-      <c r="J6" s="22">
+      <c r="I6" s="27" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="J6" s="22" t="n">
         <f>IF(I6&lt;&gt;"",(F6*I6)-G6,"")</f>
-        <v>5.5000000000000021E-2</v>
-      </c>
-      <c r="K6" s="52">
+        <v>0.04199999999999998</v>
+      </c>
+      <c r="K6" s="40" t="n">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L6" s="54">
-        <v>9.0387707575005985E-3</v>
-      </c>
-      <c r="M6" s="55">
-        <v>1.2762398410691116E-2</v>
-      </c>
-      <c r="N6" s="56">
-        <v>1.2184870170915837E-2</v>
-      </c>
-      <c r="O6" s="57">
-        <v>1.4145752430276772E-2</v>
-      </c>
-      <c r="P6" s="58">
-        <v>2.7767919668662433E-2</v>
-      </c>
-      <c r="Q6" s="59">
-        <v>4.7446096031143255E-2</v>
-      </c>
-      <c r="R6" s="60">
-        <v>4.8395504800709178E-2</v>
-      </c>
-      <c r="S6" s="61">
-        <v>9.5264236564085725E-2</v>
-      </c>
-      <c r="T6" s="62">
-        <v>5.3087804179845995E-2</v>
-      </c>
-      <c r="U6" s="50" t="s">
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="L6" s="73" t="n">
+        <v>-0.0761686279812713</v>
+      </c>
+      <c r="M6" s="74" t="n">
+        <v>-0.10904819656484875</v>
+      </c>
+      <c r="N6" s="75" t="n">
+        <v>0.14094498334364944</v>
+      </c>
+      <c r="O6" s="76" t="n">
+        <v>0.1768631652164136</v>
+      </c>
+      <c r="P6" s="77" t="n">
+        <v>0.12686435740099752</v>
+      </c>
+      <c r="Q6" s="78" t="n">
+        <v>2.755892585492447</v>
+      </c>
+      <c r="R6" s="79" t="n">
+        <v>3.5572808643531446</v>
+      </c>
+      <c r="S6" s="80" t="n">
+        <v>8.090988244199822</v>
+      </c>
+      <c r="T6" s="81" t="n">
+        <v>3.8635278667987945</v>
+      </c>
+      <c r="U6" s="38" t="s">
         <v>13</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
@@ -1318,8 +1319,8 @@
       <c r="C7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
-        <v>103</v>
+      <c r="D7" s="4" t="n">
+        <v>106.0</v>
       </c>
       <c r="E7" s="24">
         <v>1</v>
@@ -1327,54 +1328,54 @@
       <c r="F7" s="24">
         <v>0.1</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="25" t="n">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="H7" s="26"/>
-      <c r="I7" s="27">
-        <v>2.61</v>
-      </c>
-      <c r="J7" s="22">
+      <c r="I7" s="27" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="J7" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>0.161</v>
-      </c>
-      <c r="K7" s="52">
+        <v>0.139</v>
+      </c>
+      <c r="K7" s="40" t="n">
         <f t="shared" si="2"/>
-        <v>1.6099999999999999</v>
-      </c>
-      <c r="L7" s="63">
-        <v>9.1432564794632892E-3</v>
-      </c>
-      <c r="M7" s="64">
-        <v>9.7409990761278195E-3</v>
-      </c>
-      <c r="N7" s="65">
-        <v>1.1489356931052073E-2</v>
-      </c>
-      <c r="O7" s="66">
-        <v>1.5747289334920235E-2</v>
-      </c>
-      <c r="P7" s="67">
-        <v>1.2678422997512914E-2</v>
-      </c>
-      <c r="Q7" s="68">
-        <v>4.5702740306540715E-2</v>
-      </c>
-      <c r="R7" s="69">
-        <v>4.8730404916057672E-2</v>
-      </c>
-      <c r="S7" s="70">
-        <v>0</v>
-      </c>
-      <c r="T7" s="71">
-        <v>4.9661541373610445E-2</v>
+        <v>1.3900000000000001</v>
+      </c>
+      <c r="L7" s="82" t="n">
+        <v>-0.148899392483318</v>
+      </c>
+      <c r="M7" s="83" t="n">
+        <v>-0.1489200744752624</v>
+      </c>
+      <c r="N7" s="84" t="n">
+        <v>0.008774391410314024</v>
+      </c>
+      <c r="O7" s="85" t="n">
+        <v>0.298133493150404</v>
+      </c>
+      <c r="P7" s="86" t="n">
+        <v>-0.19081011101116957</v>
+      </c>
+      <c r="Q7" s="87" t="n">
+        <v>2.8707062955515528</v>
+      </c>
+      <c r="R7" s="88" t="n">
+        <v>4.068462522611122</v>
+      </c>
+      <c r="S7" s="89" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T7" s="90" t="n">
+        <v>3.5475511066256313</v>
       </c>
       <c r="U7" s="23" t="s">
         <v>15</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
@@ -1384,8 +1385,8 @@
       <c r="C8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4">
-        <v>679</v>
+      <c r="D8" s="4" t="n">
+        <v>738.0</v>
       </c>
       <c r="E8" s="24">
         <v>800</v>
@@ -1393,54 +1394,54 @@
       <c r="F8" s="24">
         <v>0.1</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="25" t="n">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>80.0</v>
       </c>
       <c r="H8" s="26"/>
-      <c r="I8" s="27">
-        <v>445.55</v>
-      </c>
-      <c r="J8" s="22">
+      <c r="I8" s="27" t="n">
+        <v>357.8</v>
+      </c>
+      <c r="J8" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>-35.444999999999993</v>
-      </c>
-      <c r="K8" s="52">
+        <v>-44.22</v>
+      </c>
+      <c r="K8" s="40" t="n">
         <f t="shared" si="2"/>
-        <v>-0.44306250000000003</v>
-      </c>
-      <c r="L8" s="72">
-        <v>0</v>
-      </c>
-      <c r="M8" s="73">
-        <v>0</v>
-      </c>
-      <c r="N8" s="74">
-        <v>0</v>
-      </c>
-      <c r="O8" s="75">
-        <v>0</v>
-      </c>
-      <c r="P8" s="76">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="77">
-        <v>0</v>
-      </c>
-      <c r="R8" s="78">
-        <v>0</v>
-      </c>
-      <c r="S8" s="79">
-        <v>0</v>
-      </c>
-      <c r="T8" s="80">
-        <v>0</v>
+        <v>-0.55275</v>
+      </c>
+      <c r="L8" s="91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="92" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="93" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="94" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="95" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q8" s="96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" s="97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T8" s="99" t="n">
+        <v>0.0</v>
       </c>
       <c r="U8" s="23" t="s">
         <v>16</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
@@ -1450,8 +1451,8 @@
       <c r="C9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4">
-        <v>87</v>
+      <c r="D9" s="4" t="n">
+        <v>93.0</v>
       </c>
       <c r="E9" s="24">
         <v>1</v>
@@ -1459,54 +1460,54 @@
       <c r="F9" s="24">
         <v>0.1</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="25" t="n">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="H9" s="26"/>
-      <c r="I9" s="27">
-        <v>0.92149999999999999</v>
-      </c>
-      <c r="J9" s="22">
+      <c r="I9" s="27" t="n">
+        <v>0.8167</v>
+      </c>
+      <c r="J9" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>-7.8499999999999959E-3</v>
-      </c>
-      <c r="K9" s="52">
+        <v>-0.01833</v>
+      </c>
+      <c r="K9" s="40" t="n">
         <f t="shared" si="2"/>
-        <v>-7.8500000000000014E-2</v>
-      </c>
-      <c r="L9" s="81">
-        <v>9.8035747674177689E-3</v>
-      </c>
-      <c r="M9" s="82">
-        <v>1.1089608622740528E-2</v>
-      </c>
-      <c r="N9" s="83">
-        <v>1.0144444449214847E-2</v>
-      </c>
-      <c r="O9" s="84">
-        <v>1.1181638553066607E-2</v>
-      </c>
-      <c r="P9" s="85">
-        <v>1.6863064486737543E-2</v>
-      </c>
-      <c r="Q9" s="86">
-        <v>3.4016119100049022E-2</v>
-      </c>
-      <c r="R9" s="87">
-        <v>4.3541971909356339E-2</v>
-      </c>
-      <c r="S9" s="88">
-        <v>0.1885830607593543</v>
-      </c>
-      <c r="T9" s="89">
-        <v>3.452195890669349E-2</v>
+        <v>-0.18330000000000002</v>
+      </c>
+      <c r="L9" s="100" t="n">
+        <v>-0.07065042465085242</v>
+      </c>
+      <c r="M9" s="101" t="n">
+        <v>-0.10565179444555767</v>
+      </c>
+      <c r="N9" s="102" t="n">
+        <v>0.013811156711854978</v>
+      </c>
+      <c r="O9" s="103" t="n">
+        <v>-0.21316258091036075</v>
+      </c>
+      <c r="P9" s="104" t="n">
+        <v>0.08802629658443152</v>
+      </c>
+      <c r="Q9" s="105" t="n">
+        <v>1.59006304410709</v>
+      </c>
+      <c r="R9" s="106" t="n">
+        <v>2.5049558625332877</v>
+      </c>
+      <c r="S9" s="107" t="n">
+        <v>17.100889352745263</v>
+      </c>
+      <c r="T9" s="108" t="n">
+        <v>2.059585875105434</v>
       </c>
       <c r="U9" s="23" t="s">
         <v>17</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
@@ -1516,8 +1517,8 @@
       <c r="C10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
-        <v>24</v>
+      <c r="D10" s="4" t="n">
+        <v>25.0</v>
       </c>
       <c r="E10" s="24">
         <v>0.125</v>
@@ -1525,54 +1526,54 @@
       <c r="F10" s="24">
         <v>0.1</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="25" t="n">
         <f t="shared" si="0"/>
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="H10" s="26"/>
-      <c r="I10" s="27">
-        <v>0.19059999999999999</v>
-      </c>
-      <c r="J10" s="22">
+      <c r="I10" s="27" t="n">
+        <v>0.1569</v>
+      </c>
+      <c r="J10" s="22" t="n">
         <f t="shared" si="1"/>
-        <v>6.5599999999999999E-3</v>
-      </c>
-      <c r="K10" s="52">
+        <v>0.003190000000000002</v>
+      </c>
+      <c r="K10" s="40" t="n">
         <f t="shared" si="2"/>
-        <v>0.52479999999999993</v>
-      </c>
-      <c r="L10" s="90">
-        <v>9.7155212792599151E-3</v>
-      </c>
-      <c r="M10" s="91">
-        <v>1.1009220308649788E-2</v>
-      </c>
-      <c r="N10" s="92">
-        <v>1.0385016023763707E-2</v>
-      </c>
-      <c r="O10" s="93">
-        <v>1.5647735807109556E-2</v>
-      </c>
-      <c r="P10" s="94">
-        <v>3.6127393605678786E-2</v>
-      </c>
-      <c r="Q10" s="95">
-        <v>3.9335806852520444E-2</v>
-      </c>
-      <c r="R10" s="96">
-        <v>1.4979302470626106E-2</v>
-      </c>
-      <c r="S10" s="97">
-        <v>3.8466063789488511E-2</v>
-      </c>
-      <c r="T10" s="98">
-        <v>3.9688852721455885E-2</v>
+        <v>0.2552000000000001</v>
+      </c>
+      <c r="L10" s="109" t="n">
+        <v>-0.24889287096410356</v>
+      </c>
+      <c r="M10" s="110" t="n">
+        <v>-0.16987429918132363</v>
+      </c>
+      <c r="N10" s="111" t="n">
+        <v>-0.1355646710294664</v>
+      </c>
+      <c r="O10" s="112" t="n">
+        <v>0.16641709008449596</v>
+      </c>
+      <c r="P10" s="113" t="n">
+        <v>1.757659711821924</v>
+      </c>
+      <c r="Q10" s="114" t="n">
+        <v>1.5119924022236177</v>
+      </c>
+      <c r="R10" s="115" t="n">
+        <v>0.22570789904291685</v>
+      </c>
+      <c r="S10" s="116" t="n">
+        <v>2.4461718499814844</v>
+      </c>
+      <c r="T10" s="117" t="n">
+        <v>2.2671463756539505</v>
       </c>
       <c r="U10" s="23" t="s">
         <v>14</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
@@ -1588,19 +1589,19 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K11" s="52" t="str">
+      <c r="K11" s="40" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="48"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="51"/>
       <c r="U11" s="23"/>
       <c r="V11" s="4" t="s">
         <v>25</v>
@@ -1619,19 +1620,19 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K12" s="52" t="str">
+      <c r="K12" s="40" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="48"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="51"/>
       <c r="U12" s="23"/>
       <c r="V12" s="4" t="s">
         <v>25</v>
@@ -1650,19 +1651,19 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="53" t="str">
+      <c r="K13" s="41" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="49"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
+      <c r="T13" s="53"/>
       <c r="U13" s="37"/>
       <c r="V13" s="29" t="s">
         <v>25</v>

</xml_diff>